<commit_message>
Update Detailed Protein Dataset.xlsx
</commit_message>
<xml_diff>
--- a/data/Detailed Protein Dataset.xlsx
+++ b/data/Detailed Protein Dataset.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadel\Desktop\Rapport de stage MI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadel\Documents\GitHub\AlphaFold3-vs-ESMFold-OmegaFold-Benchmark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9078BA2-8162-437B-8FB2-A3A7BC9C680F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED321D3-7C2C-4A76-A8AA-D4A069896E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
   <si>
     <t>MGYP000261684433</t>
   </si>
@@ -352,130 +351,13 @@
   </si>
   <si>
     <t>RBD de SARS-CoV-2 + 3 Fab anticorps (S2E12, S309, S304)</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>MSA</t>
-  </si>
-  <si>
-    <t>AF3 RMSD (complex)</t>
-  </si>
-  <si>
-    <t>Octamer</t>
-  </si>
-  <si>
-    <t>Shallow</t>
-  </si>
-  <si>
-    <t>26.067</t>
-  </si>
-  <si>
-    <t>0.311</t>
-  </si>
-  <si>
-    <t>0.434</t>
-  </si>
-  <si>
-    <t>ESMFold</t>
-  </si>
-  <si>
-    <t>Dimer</t>
-  </si>
-  <si>
-    <t>8.746</t>
-  </si>
-  <si>
-    <t>0.492</t>
-  </si>
-  <si>
-    <t>0.825</t>
-  </si>
-  <si>
-    <t>Tetramer</t>
-  </si>
-  <si>
-    <t>13.645</t>
-  </si>
-  <si>
-    <t>0.509</t>
-  </si>
-  <si>
-    <t>0.522</t>
-  </si>
-  <si>
-    <t>0.597</t>
-  </si>
-  <si>
-    <t>0.809</t>
-  </si>
-  <si>
-    <t>5.359</t>
-  </si>
-  <si>
-    <t>AlphaFold3</t>
-  </si>
-  <si>
-    <t>Hetero</t>
-  </si>
-  <si>
-    <t>27.765</t>
-  </si>
-  <si>
-    <t>1.679</t>
-  </si>
-  <si>
-    <t>1.011</t>
-  </si>
-  <si>
-    <t>OmegaFold</t>
-  </si>
-  <si>
-    <t>Hemoglobin</t>
-  </si>
-  <si>
-    <t>0.480</t>
-  </si>
-  <si>
-    <t>0.297</t>
-  </si>
-  <si>
-    <t>0.379</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESMFold </t>
-  </si>
-  <si>
-    <t>Hetero-7-mer</t>
-  </si>
-  <si>
-    <t>0.364</t>
-  </si>
-  <si>
-    <t>0.308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.098 </t>
-  </si>
-  <si>
-    <t>ESM RMSD (chain A or D)</t>
-  </si>
-  <si>
-    <t>OF RMSD (chain A or D)</t>
-  </si>
-  <si>
-    <t>Best (chain A or D)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,41 +394,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,18 +426,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95B3D7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCD5B4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -761,7 +598,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
@@ -808,20 +645,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1601,203 +1424,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D1089E-5137-4A6B-B3E0-ECEB82860621}">
-  <dimension ref="C4:I11"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="4" spans="3:9" ht="56" x14ac:dyDescent="0.35">
-      <c r="C4" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C9" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>